<commit_message>
day 14: Improve conditional formatting
</commit_message>
<xml_diff>
--- a/2019/day_14.xlsx
+++ b/2019/day_14.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="40960" windowHeight="25140"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,114 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -466,6 +573,16 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -692,7 +809,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2375,7 +2492,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" state="frozen"/>
-      <selection activeCell="AB27" sqref="AB27"/>
+      <selection activeCell="L50" sqref="L50"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
@@ -17143,7 +17260,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:BI60">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -17167,7 +17284,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" state="frozen"/>
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="G9" sqref="G9"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -26875,6 +26992,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:AG60">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
@@ -26887,7 +27012,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" state="frozen"/>
-      <selection activeCell="AH1" sqref="AH1:AH1048576"/>
+      <selection activeCell="K24" sqref="K24"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -36596,6 +36721,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:AG60">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>

</xml_diff>